<commit_message>
Hotfix for point mass velocity issue
V registers inf for 0 TPS for about 20 values of endurance--even on old stable versions
</commit_message>
<xml_diff>
--- a/custom sim/track_files/Michigan_2021_Endurance.xlsx
+++ b/custom sim/track_files/Michigan_2021_Endurance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Westo\Documents\FEB Personal\Open-Lap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\FEBSim\custom sim\track_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8FAF87-099C-4D10-ABF7-EC0127084D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62092139-8317-487B-99DF-8B6F4F59AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -279,7 +279,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -287,15 +287,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -358,6 +349,15 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -375,27 +375,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C134" totalsRowCount="1">
   <autoFilter ref="A1:C133" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Section Length" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Corner Radius" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Section Length" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Corner Radius" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:B1048576" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:B1048576" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:B1048576" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Point [m]" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Elevation [m]" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Point [m]" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Elevation [m]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:B3" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:B3" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
   <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start Point [m]"/>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S74" sqref="S74"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>